<commit_message>
moved logic of finding answer to a method named get_answer
</commit_message>
<xml_diff>
--- a/gptdata.xlsx
+++ b/gptdata.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ChatGPT ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEF82BB-3DB5-425C-86D5-3E1C9FCF7A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD3992B-543E-48FE-A4E5-96E40DFE1442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" tabRatio="762" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" tabRatio="762" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relevance" sheetId="4" r:id="rId1"/>
     <sheet name="RelevanceTypes" sheetId="8" r:id="rId2"/>
-    <sheet name="Basic" sheetId="1" r:id="rId3"/>
-    <sheet name="Location" sheetId="2" r:id="rId4"/>
-    <sheet name="Colleges" sheetId="3" r:id="rId5"/>
-    <sheet name="Faculty" sheetId="5" r:id="rId6"/>
+    <sheet name="Location" sheetId="2" r:id="rId3"/>
+    <sheet name="Basic" sheetId="1" r:id="rId4"/>
+    <sheet name="Faculty" sheetId="5" r:id="rId5"/>
+    <sheet name="Colleges" sheetId="3" r:id="rId6"/>
     <sheet name="DataSheet" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="117">
   <si>
     <t>Question</t>
   </si>
@@ -81,9 +81,6 @@
     <t>visakhapatnam</t>
   </si>
   <si>
-    <t>Architecture, Civil, Computer Science, Information Technology, Chemical, Electrical, Electronics, Mechanical, Geo Informatics, Marine</t>
-  </si>
-  <si>
     <t>Department</t>
   </si>
   <si>
@@ -297,12 +294,6 @@
     <t>There are $Count departments in $College.</t>
   </si>
   <si>
-    <t>There are $Count faculty members in $Department of $College.</t>
-  </si>
-  <si>
-    <t>$Name is currently working as $Designation in $Department of $College.</t>
-  </si>
-  <si>
     <t>AU Andhra University located</t>
   </si>
   <si>
@@ -321,9 +312,6 @@
     <t>What are they? List them colleges</t>
   </si>
   <si>
-    <t>Departments AU College Engineering</t>
-  </si>
-  <si>
     <t>hi hello hey</t>
   </si>
   <si>
@@ -360,9 +348,6 @@
     <t>faculty list</t>
   </si>
   <si>
-    <t>faculty profile</t>
-  </si>
-  <si>
     <t>College,Department</t>
   </si>
   <si>
@@ -375,9 +360,6 @@
     <t>Following are the departments present in $College.$NL$List</t>
   </si>
   <si>
-    <t>Following are the faculty present in $Department of $College.$NL$List</t>
-  </si>
-  <si>
     <t>who you name your</t>
   </si>
   <si>
@@ -387,7 +369,19 @@
     <t>Professor &amp; Co-ordinator, IQAC, Chairperson, Board of Studies</t>
   </si>
   <si>
-    <t>departments profile details prof faculty college department</t>
+    <t>There are $Count faculty members in $Department department of $College.</t>
+  </si>
+  <si>
+    <t>Following are the faculty present in $Department department of $College.$NL$List</t>
+  </si>
+  <si>
+    <t>$Name is currently working as $Designation in $Department department of $College.</t>
+  </si>
+  <si>
+    <t>faculty profile about</t>
+  </si>
+  <si>
+    <t>departments profile details prof faculty college department about</t>
   </si>
 </sst>
 </file>
@@ -718,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF7F9EB-044B-432F-A76C-B9394198BD95}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -738,7 +732,7 @@
     </row>
     <row r="2" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -754,10 +748,10 @@
     </row>
     <row r="4" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -792,7 +786,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -800,7 +794,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -808,15 +802,15 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -825,136 +819,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="44.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA7EAF6-D767-4C93-9528-F87E2BDAF5FF}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -982,7 +846,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -993,13 +857,143 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="44.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1008,64 +1002,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF375775-692B-46A2-B001-F734C853D46A}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="170.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B483AEFF-F926-4EE7-93DE-F8263CE1F8BB}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1080,372 +1021,414 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
       <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>39</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>40</v>
-      </c>
-      <c r="F9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
         <v>42</v>
       </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>43</v>
-      </c>
-      <c r="F10" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
         <v>45</v>
-      </c>
-      <c r="D11" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" t="s">
         <v>51</v>
-      </c>
-      <c r="D12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
         <v>53</v>
-      </c>
-      <c r="D13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" t="s">
         <v>56</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
         <v>57</v>
-      </c>
-      <c r="E14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" t="s">
         <v>59</v>
-      </c>
-      <c r="D15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" t="s">
         <v>61</v>
-      </c>
-      <c r="D16" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" t="s">
         <v>63</v>
-      </c>
-      <c r="D17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
         <v>65</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" t="s">
         <v>66</v>
-      </c>
-      <c r="E18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
         <v>47</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" t="s">
         <v>48</v>
-      </c>
-      <c r="E19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF375775-692B-46A2-B001-F734C853D46A}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="170.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1454,7 +1437,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1462,7 +1445,7 @@
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="64.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="71.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1471,137 +1454,137 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" t="s">
         <v>84</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>85</v>
       </c>
-      <c r="F1" t="s">
-        <v>86</v>
-      </c>
       <c r="G1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated data in excel sheet
</commit_message>
<xml_diff>
--- a/gptdata.xlsx
+++ b/gptdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ChatGPT ML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SmartGPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD3992B-543E-48FE-A4E5-96E40DFE1442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAC49FA-39A9-42D0-9E9B-37FB712D97C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" tabRatio="762" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="762" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relevance" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="121">
   <si>
     <t>Question</t>
   </si>
@@ -318,24 +318,12 @@
     <t>I am named SmartGPT by my creator Anjani Sowmya.</t>
   </si>
   <si>
-    <t>I do help people in finding answers to their questions.</t>
-  </si>
-  <si>
     <t>Hello. Nice to meet you.</t>
   </si>
   <si>
     <t>what you</t>
   </si>
   <si>
-    <t>who VC Vice Chancellor AU Andhra University</t>
-  </si>
-  <si>
-    <t>who Registrar AU Andhra University</t>
-  </si>
-  <si>
-    <t>who Rector AU Andhra University</t>
-  </si>
-  <si>
     <t>list departments</t>
   </si>
   <si>
@@ -363,9 +351,6 @@
     <t>who you name your</t>
   </si>
   <si>
-    <t>hi hello hey located established vice chancellor vc registrar rector colleges where au andhra university who how what your</t>
-  </si>
-  <si>
     <t>Professor &amp; Co-ordinator, IQAC, Chairperson, Board of Studies</t>
   </si>
   <si>
@@ -382,6 +367,33 @@
   </si>
   <si>
     <t>departments profile details prof faculty college department about</t>
+  </si>
+  <si>
+    <t>are you smart</t>
+  </si>
+  <si>
+    <t>I am getting smarter day by day ;-)</t>
+  </si>
+  <si>
+    <t>hi hello hey located established vice chancellor vc registrar rector colleges where au andhra university who how what your smart introduce yourself</t>
+  </si>
+  <si>
+    <t>introduce yourself</t>
+  </si>
+  <si>
+    <t>I do help people in finding answers to the questions.</t>
+  </si>
+  <si>
+    <t>Hello, I am SmartGPT. I do help people in finding answers to the questions. I am learning new things and getting smarter day by day ;-)</t>
+  </si>
+  <si>
+    <t>VC Vice Chancellor AU Andhra University</t>
+  </si>
+  <si>
+    <t>Registrar AU Andhra University</t>
+  </si>
+  <si>
+    <t>Rector AU Andhra University</t>
   </si>
 </sst>
 </file>
@@ -712,13 +724,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF7F9EB-044B-432F-A76C-B9394198BD95}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="102.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="123.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -732,7 +744,7 @@
     </row>
     <row r="2" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -748,7 +760,7 @@
     </row>
     <row r="4" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
         <v>72</v>
@@ -873,17 +885,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="44.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="111.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -905,12 +917,12 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -921,78 +933,100 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>89</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1215,7 +1249,7 @@
         <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E11" t="s">
         <v>39</v>
@@ -1469,12 +1503,12 @@
         <v>85</v>
       </c>
       <c r="G1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>77</v>
@@ -1497,7 +1531,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
         <v>76</v>
@@ -1512,7 +1546,7 @@
         <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
@@ -1520,7 +1554,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
         <v>75</v>
@@ -1532,10 +1566,10 @@
         <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
@@ -1543,7 +1577,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
         <v>78</v>
@@ -1555,10 +1589,10 @@
         <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
@@ -1566,7 +1600,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
         <v>74</v>
@@ -1578,10 +1612,10 @@
         <v>72</v>
       </c>
       <c r="E6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F6" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G6" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
added information about AU in basic relevane
</commit_message>
<xml_diff>
--- a/gptdata.xlsx
+++ b/gptdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SmartGPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAC49FA-39A9-42D0-9E9B-37FB712D97C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9516A8-414D-406F-99F4-D1B5FB794456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="762" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="762" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relevance" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="123">
   <si>
     <t>Question</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Visakhapatnam is famous for its beautiful beaches, natural harbour, steel plant, araku valley and many more.</t>
   </si>
   <si>
-    <t>Andhra University was established in 1926.</t>
-  </si>
-  <si>
     <t>Prof. V. Krishna Mohan is the Registrar of Andhra University.</t>
   </si>
   <si>
@@ -375,9 +372,6 @@
     <t>I am getting smarter day by day ;-)</t>
   </si>
   <si>
-    <t>hi hello hey located established vice chancellor vc registrar rector colleges where au andhra university who how what your smart introduce yourself</t>
-  </si>
-  <si>
     <t>introduce yourself</t>
   </si>
   <si>
@@ -394,6 +388,18 @@
   </si>
   <si>
     <t>Rector AU Andhra University</t>
+  </si>
+  <si>
+    <t>know about AU Andhra University</t>
+  </si>
+  <si>
+    <t>hi hello hey located established vice chancellor vc registrar rector colleges where au andhra university who how what your smart introduce yourself do know about</t>
+  </si>
+  <si>
+    <t>Andhra University is one of the oldest educational institutions in the country and also the first university to be conceived as a residential and teaching-cum-affiliating University, mainly devoted to post-graduate teaching and research. Andhra University was constituted in the year 1926 by the Madras Act of 1926. The 94-year-old institution is fortunate to have Sir C.R. Reddy as its founder Vice-Chancellor, as the steps taken by this visionary proved to be fruitful in the long run. Former President of India Dr. Sarvepalli Radhakrishnan was one of its Vice-Chancellors who succeed Dr. C. R. Reddy in 1931. The leaders of the university always believed that excellence in higher education is the best investment for the country and engaged the services of famous educationists such as Dr. T.R. Seshadri, Dr. S. Bhagavantham, Professor Hiren Mukherjee, Professor Humayan Kabir and Dr. V.K.R.V. Rao, to mention a few who set high standards for teaching and research. Nobel Lariat C V Raman was the proud alumnus of the University and closely associated in laying research foundations in Physics. Padmavibhushan Prof. C R Rao, the renowned statistician of the world, was also the proud alumnus of the University. Ever since its inception in 1926 Andhra University has an impeccable record of catering to the educational needs and solving the sociological problems of the region. The University is relentless in its efforts in maintaining standards in teaching and research, ensuring proper character building and development among the students, encouraging community developmental programmes, nurturing leadership in young men and women and imbibing a sense of responsibility to become good citizens, while striving for excellence in all fronts.</t>
+  </si>
+  <si>
+    <t>Andhra University was established in 1926 by the Madras Act of 1926. The 94-year-old institution is fortunate to have Sir C.R. Reddy as its founder Vice-Chancellor, as the steps taken by this visionary proved to be fruitful in the long run.</t>
   </si>
 </sst>
 </file>
@@ -744,7 +750,7 @@
     </row>
     <row r="2" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -752,7 +758,7 @@
     </row>
     <row r="3" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -760,10 +766,10 @@
     </row>
     <row r="4" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -798,7 +804,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -806,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -814,15 +820,15 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -858,7 +864,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -869,7 +875,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -885,10 +891,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -911,62 +917,62 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -977,18 +983,18 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -999,18 +1005,18 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -1021,7 +1027,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -1030,8 +1036,20 @@
         <v>10</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1055,367 +1073,367 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
       <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>39</v>
-      </c>
-      <c r="F9" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
         <v>41</v>
       </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>42</v>
-      </c>
-      <c r="F10" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
         <v>44</v>
-      </c>
-      <c r="D11" t="s">
-        <v>106</v>
-      </c>
-      <c r="E11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
         <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
         <v>52</v>
-      </c>
-      <c r="D13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
         <v>55</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
         <v>56</v>
-      </c>
-      <c r="E14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
         <v>58</v>
-      </c>
-      <c r="D15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s">
         <v>60</v>
-      </c>
-      <c r="D16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" t="s">
         <v>62</v>
-      </c>
-      <c r="D17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
         <v>64</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" t="s">
         <v>65</v>
-      </c>
-      <c r="E18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
         <v>46</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" t="s">
         <v>47</v>
-      </c>
-      <c r="E19" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1452,13 +1470,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1488,137 +1506,137 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
         <v>83</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>84</v>
       </c>
-      <c r="F1" t="s">
-        <v>85</v>
-      </c>
       <c r="G1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" t="s">
         <v>100</v>
       </c>
-      <c r="B5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" t="s">
-        <v>101</v>
-      </c>
       <c r="F5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>